<commit_message>
pull controlled vocabulary from MetadataDictionary
</commit_message>
<xml_diff>
--- a/Data/MetadataDictionary.xlsx
+++ b/Data/MetadataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rscully\Documents\Projects\Habitat Data Sharing\2019_2020\Code\Stream-Monitoring-Data-Exchange-Specifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D028818-4258-4595-BB08-F5D817C7F3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A47AA6-6778-4010-B413-11B0FE4E0A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34695" yWindow="5145" windowWidth="19200" windowHeight="14655" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
+    <workbookView xWindow="-38520" yWindow="-4305" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="MetadataDict" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="348">
   <si>
     <t>entity</t>
   </si>
@@ -1076,6 +1076,9 @@
   </si>
   <si>
     <t>Nephelometric Turbidity unit</t>
+  </si>
+  <si>
+    <t>A unique numeric identifier assigned to the measurementType Sin.</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6029B-A891-4391-9A91-8B6BC1C75C07}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
@@ -2930,9 +2933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063D4566-F61A-451E-B178-010037E4B35B}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B193" sqref="B193"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4889,7 +4892,7 @@
         <v>500</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>273</v>
+        <v>347</v>
       </c>
       <c r="E105" t="s">
         <v>13</v>
@@ -7039,26 +7042,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Number xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
-    <DateandTime xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006688A6CBE26CBF41BFE362BEC34502BA" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="916ec95d980b70225c2beeb175eb34ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xmlns:ns3="3618cbaa-901d-4c6b-9f1a-f53e3aa15701" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1086361ad164fb1fc8fad31a5b69396c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7296,26 +7279,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Number xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
+    <DateandTime xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783B9ED7-A86D-4C20-8581-4B66EC9EBDC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7333,4 +7317,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update to use EmunDict to build controlled vocabulary
</commit_message>
<xml_diff>
--- a/Data/MetadataDictionary.xlsx
+++ b/Data/MetadataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rscully\Documents\Projects\Habitat Data Sharing\2019_2020\Code\Stream-Monitoring-Data-Exchange-Specifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A47AA6-6778-4010-B413-11B0FE4E0A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BEE017-D0F1-4E16-AF52-B5BA3E92F075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-4305" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
+    <workbookView xWindow="-38520" yWindow="-4305" windowWidth="38640" windowHeight="21240" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="MetadataDict" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="351">
   <si>
     <t>entity</t>
   </si>
@@ -412,9 +412,6 @@
     <t>45, "20", "1", "14.5", "UV-light"</t>
   </si>
   <si>
-    <t>ODM2.Results.MeasurementResults</t>
-  </si>
-  <si>
     <t>DataMapping</t>
   </si>
   <si>
@@ -1079,6 +1076,18 @@
   </si>
   <si>
     <t>A unique numeric identifier assigned to the measurementType Sin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examples </t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">termID </t>
+  </si>
+  <si>
+    <t>RecordLevel</t>
   </si>
 </sst>
 </file>
@@ -1503,16 +1512,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6029B-A891-4391-9A91-8B6BC1C75C07}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.7265625" customWidth="1"/>
     <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.90625" style="3" customWidth="1"/>
     <col min="4" max="4" width="7.26953125" customWidth="1"/>
     <col min="5" max="5" width="6.453125" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" customWidth="1"/>
@@ -1521,11 +1530,11 @@
     <col min="9" max="9" width="7" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.453125" style="1" customWidth="1"/>
     <col min="11" max="12" width="10.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27" style="7" customWidth="1"/>
-    <col min="14" max="14" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" style="7" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1559,13 +1568,22 @@
       <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="13"/>
-    </row>
-    <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="L1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -1576,9 +1594,9 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1598,10 +1616,13 @@
       <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1628,10 +1649,13 @@
       <c r="N4" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1657,10 +1681,13 @@
       <c r="N5" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -1689,10 +1716,13 @@
       <c r="N6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -1715,10 +1745,13 @@
       <c r="N7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -1738,10 +1771,13 @@
       <c r="N8" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
@@ -1767,10 +1803,13 @@
       <c r="N9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
@@ -1793,10 +1832,13 @@
       <c r="N10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -1819,8 +1861,11 @@
       <c r="N11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O11">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1831,7 +1876,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1850,8 +1895,11 @@
       <c r="L13" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1879,8 +1927,11 @@
       <c r="N14" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O14">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1905,8 +1956,11 @@
       <c r="N15" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O15">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1934,8 +1988,11 @@
       <c r="N16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O16">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1963,8 +2020,11 @@
       <c r="N17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O17">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1986,8 +2046,11 @@
       <c r="N18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O18">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2018,8 +2081,11 @@
       <c r="N19" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O19">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2047,8 +2113,11 @@
       <c r="N20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="63.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O20">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="63.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -2059,7 +2128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -2081,8 +2150,11 @@
       <c r="L22" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2116,8 +2188,11 @@
       <c r="N23" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="O23">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2145,8 +2220,11 @@
       <c r="N24" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O24">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -2177,8 +2255,11 @@
       <c r="N25" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2206,8 +2287,11 @@
       <c r="N26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O26">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="33.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -2238,8 +2322,11 @@
       <c r="N27" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O27">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2267,8 +2354,11 @@
       <c r="N28" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O28">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2299,8 +2389,11 @@
       <c r="N29" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="O29">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -2311,7 +2404,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2336,8 +2429,11 @@
       <c r="N31" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -2361,6 +2457,9 @@
       </c>
       <c r="N32" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="O32">
+        <v>400</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
@@ -2388,6 +2487,9 @@
       <c r="N33" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="O33">
+        <v>403</v>
+      </c>
     </row>
     <row r="34" spans="1:15" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
@@ -2405,6 +2507,9 @@
       <c r="I34" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="O34">
+        <v>401</v>
+      </c>
     </row>
     <row r="35" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -2431,30 +2536,30 @@
       <c r="N35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O35" t="s">
-        <v>125</v>
+      <c r="O35">
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" t="s">
         <v>127</v>
       </c>
-      <c r="G36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G37" t="s">
         <v>13</v>
@@ -2463,15 +2568,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="G38" t="s">
         <v>13</v>
@@ -2480,15 +2585,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
         <v>119</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G39" t="s">
         <v>13</v>
@@ -2500,18 +2605,21 @@
         <v>34</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+      <c r="O39">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G40" t="s">
         <v>13</v>
@@ -2523,18 +2631,21 @@
         <v>22</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="O40">
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
         <v>136</v>
-      </c>
-      <c r="C41" t="s">
-        <v>137</v>
       </c>
       <c r="G41" t="s">
         <v>13</v>
@@ -2545,13 +2656,13 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
         <v>138</v>
-      </c>
-      <c r="C42" t="s">
-        <v>139</v>
       </c>
       <c r="G42" t="s">
         <v>13</v>
@@ -2562,13 +2673,13 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" t="s">
         <v>140</v>
-      </c>
-      <c r="C43" t="s">
-        <v>141</v>
       </c>
       <c r="G43" t="s">
         <v>13</v>
@@ -2577,18 +2688,18 @@
         <v>21</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
         <v>143</v>
-      </c>
-      <c r="C44" t="s">
-        <v>144</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
@@ -2600,18 +2711,18 @@
         <v>34</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" t="s">
         <v>146</v>
-      </c>
-      <c r="C45" t="s">
-        <v>147</v>
       </c>
       <c r="G45" t="s">
         <v>13</v>
@@ -2625,13 +2736,13 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s">
         <v>148</v>
-      </c>
-      <c r="C46" t="s">
-        <v>149</v>
       </c>
       <c r="G46" t="s">
         <v>13</v>
@@ -2643,18 +2754,18 @@
         <v>34</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
+        <v>150</v>
+      </c>
+      <c r="C47" t="s">
         <v>151</v>
-      </c>
-      <c r="C47" t="s">
-        <v>152</v>
       </c>
       <c r="G47" t="s">
         <v>13</v>
@@ -2666,29 +2777,29 @@
         <v>34</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="58" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" t="s">
         <v>155</v>
       </c>
-      <c r="G48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="G49" t="s">
         <v>13</v>
@@ -2697,15 +2808,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G50" t="s">
         <v>13</v>
@@ -2717,15 +2828,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="G51" t="s">
         <v>13</v>
@@ -2734,15 +2845,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G52" t="s">
         <v>13</v>
@@ -2753,13 +2864,13 @@
     </row>
     <row r="53" spans="1:12" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
         <v>116</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G53" t="s">
         <v>13</v>
@@ -2773,13 +2884,13 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" t="s">
         <v>160</v>
-      </c>
-      <c r="C54" t="s">
-        <v>161</v>
       </c>
       <c r="G54" t="s">
         <v>13</v>
@@ -2793,13 +2904,13 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" t="s">
         <v>162</v>
-      </c>
-      <c r="C55" t="s">
-        <v>163</v>
       </c>
       <c r="G55" t="s">
         <v>13</v>
@@ -2811,7 +2922,7 @@
         <v>34</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L55" s="1" t="s">
         <v>28</v>
@@ -2819,13 +2930,13 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" t="s">
         <v>136</v>
-      </c>
-      <c r="C56" t="s">
-        <v>137</v>
       </c>
       <c r="G56" t="s">
         <v>13</v>
@@ -2839,13 +2950,13 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B57" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" t="s">
         <v>165</v>
-      </c>
-      <c r="C57" t="s">
-        <v>166</v>
       </c>
       <c r="G57" t="s">
         <v>13</v>
@@ -2859,13 +2970,13 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" t="s">
         <v>167</v>
-      </c>
-      <c r="C58" t="s">
-        <v>168</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
@@ -2877,7 +2988,7 @@
         <v>34</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L58" s="1" t="s">
         <v>28</v>
@@ -2885,13 +2996,13 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59" t="s">
         <v>170</v>
-      </c>
-      <c r="C59" t="s">
-        <v>171</v>
       </c>
       <c r="G59" t="s">
         <v>13</v>
@@ -2902,13 +3013,13 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
+        <v>171</v>
+      </c>
+      <c r="C60" t="s">
         <v>172</v>
-      </c>
-      <c r="C60" t="s">
-        <v>173</v>
       </c>
       <c r="G60" t="s">
         <v>13</v>
@@ -2920,7 +3031,7 @@
         <v>34</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2933,9 +3044,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063D4566-F61A-451E-B178-010037E4B35B}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2959,7 +3070,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>6</v>
@@ -2967,8 +3078,12 @@
       <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="G1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -2982,7 +3097,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -3000,7 +3115,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -3018,7 +3133,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -3036,7 +3151,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -3047,7 +3162,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -3070,7 +3185,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -3085,10 +3200,10 @@
         <v>institutionCode</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
         <v>182</v>
-      </c>
-      <c r="D8" t="s">
-        <v>183</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -3103,10 +3218,10 @@
         <v>institutionCode</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" t="s">
         <v>184</v>
-      </c>
-      <c r="D9" t="s">
-        <v>185</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -3121,10 +3236,10 @@
         <v>institutionCode</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" t="s">
         <v>186</v>
-      </c>
-      <c r="D10" t="s">
-        <v>187</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -3156,10 +3271,10 @@
         <v>projectCode</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" t="s">
         <v>188</v>
-      </c>
-      <c r="D12" t="s">
-        <v>189</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -3174,10 +3289,10 @@
         <v>projectCode</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" t="s">
         <v>190</v>
-      </c>
-      <c r="D13" t="s">
-        <v>191</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -3192,10 +3307,10 @@
         <v>projectCode</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" t="s">
         <v>192</v>
-      </c>
-      <c r="D14" t="s">
-        <v>193</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -3210,10 +3325,10 @@
         <v>projectCode</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" t="s">
         <v>194</v>
-      </c>
-      <c r="D15" t="s">
-        <v>195</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -3231,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -3249,7 +3364,7 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -3267,7 +3382,7 @@
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -3285,7 +3400,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -3300,10 +3415,10 @@
         <v>locationRemarks</v>
       </c>
       <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D20" t="s">
         <v>196</v>
-      </c>
-      <c r="D20" t="s">
-        <v>197</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -3318,10 +3433,10 @@
         <v>locationRemarks</v>
       </c>
       <c r="C21" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" t="s">
         <v>198</v>
-      </c>
-      <c r="D21" t="s">
-        <v>199</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -3336,10 +3451,10 @@
         <v>siteSelectionType</v>
       </c>
       <c r="C22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" t="s">
         <v>200</v>
-      </c>
-      <c r="D22" t="s">
-        <v>201</v>
       </c>
       <c r="E22" t="s">
         <v>106</v>
@@ -3354,10 +3469,10 @@
         <v>siteSelectionType</v>
       </c>
       <c r="C23" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -3372,10 +3487,10 @@
         <v>siteSelectionType</v>
       </c>
       <c r="C24" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" t="s">
         <v>204</v>
-      </c>
-      <c r="D24" t="s">
-        <v>205</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -3406,7 +3521,7 @@
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D26" t="s">
         <v>78</v>
@@ -3458,10 +3573,10 @@
         <v>fieldNotes</v>
       </c>
       <c r="C29" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" t="s">
         <v>207</v>
-      </c>
-      <c r="D29" t="s">
-        <v>208</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -3476,10 +3591,10 @@
         <v>fieldNotes</v>
       </c>
       <c r="C30" t="s">
+        <v>208</v>
+      </c>
+      <c r="D30" t="s">
         <v>209</v>
-      </c>
-      <c r="D30" t="s">
-        <v>210</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -3494,10 +3609,10 @@
         <v>fieldNotes</v>
       </c>
       <c r="C31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D31" t="s">
         <v>211</v>
-      </c>
-      <c r="D31" t="s">
-        <v>212</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -3529,10 +3644,10 @@
         <v>samplingProtocol</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -3581,10 +3696,10 @@
         <v>beaverImpactFlow</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" t="s">
         <v>215</v>
-      </c>
-      <c r="D36" t="s">
-        <v>216</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -3599,10 +3714,10 @@
         <v>beaverImpactFlow</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D37" t="s">
         <v>217</v>
-      </c>
-      <c r="D37" t="s">
-        <v>218</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -3617,10 +3732,10 @@
         <v>measurementType</v>
       </c>
       <c r="C38" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -3636,10 +3751,10 @@
         <v>measurementType</v>
       </c>
       <c r="C39" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -3655,10 +3770,10 @@
         <v>measurementType</v>
       </c>
       <c r="C40" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -3674,10 +3789,10 @@
         <v>measurementType</v>
       </c>
       <c r="C41" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -3693,10 +3808,10 @@
         <v>measurementType</v>
       </c>
       <c r="C42" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -3712,10 +3827,10 @@
         <v>measurementType</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -3731,10 +3846,10 @@
         <v>measurementType</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -3750,10 +3865,10 @@
         <v>measurementType</v>
       </c>
       <c r="C45" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -3769,10 +3884,10 @@
         <v>measurementType</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" t="s">
         <v>235</v>
-      </c>
-      <c r="D46" t="s">
-        <v>236</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -3788,10 +3903,10 @@
         <v>measurementType</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -3807,10 +3922,10 @@
         <v>measurementType</v>
       </c>
       <c r="C48" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D48" t="s">
         <v>239</v>
-      </c>
-      <c r="D48" t="s">
-        <v>240</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -3826,10 +3941,10 @@
         <v>measurementType</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -3845,10 +3960,10 @@
         <v>measurementType</v>
       </c>
       <c r="C50" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D50" t="s">
         <v>243</v>
-      </c>
-      <c r="D50" t="s">
-        <v>244</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -3864,10 +3979,10 @@
         <v>measurementType</v>
       </c>
       <c r="C51" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -3883,10 +3998,10 @@
         <v>measurementType</v>
       </c>
       <c r="C52" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D52" t="s">
         <v>247</v>
-      </c>
-      <c r="D52" t="s">
-        <v>248</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -3902,10 +4017,10 @@
         <v>measurementType</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>250</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -3921,10 +4036,10 @@
         <v>measurementType</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D54" t="s">
         <v>251</v>
-      </c>
-      <c r="D54" t="s">
-        <v>252</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -3940,10 +4055,10 @@
         <v>measurementType</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D55" t="s">
         <v>253</v>
-      </c>
-      <c r="D55" t="s">
-        <v>254</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -3959,10 +4074,10 @@
         <v>measurementType</v>
       </c>
       <c r="C56" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D56" t="s">
         <v>255</v>
-      </c>
-      <c r="D56" t="s">
-        <v>256</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -3978,10 +4093,10 @@
         <v>measurementType</v>
       </c>
       <c r="C57" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D57" t="s">
         <v>257</v>
-      </c>
-      <c r="D57" t="s">
-        <v>258</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -3997,10 +4112,10 @@
         <v>measurementType</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D58" t="s">
         <v>259</v>
-      </c>
-      <c r="D58" t="s">
-        <v>260</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -4016,10 +4131,10 @@
         <v>measurementType</v>
       </c>
       <c r="C59" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -4035,10 +4150,10 @@
         <v>measurementType</v>
       </c>
       <c r="C60" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D60" t="s">
         <v>263</v>
-      </c>
-      <c r="D60" t="s">
-        <v>264</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -4054,10 +4169,10 @@
         <v>measurementType</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D61" t="s">
         <v>265</v>
-      </c>
-      <c r="D61" t="s">
-        <v>266</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -4073,10 +4188,10 @@
         <v>measurementType</v>
       </c>
       <c r="C62" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D62" t="s">
         <v>267</v>
-      </c>
-      <c r="D62" t="s">
-        <v>268</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -4092,10 +4207,10 @@
         <v>measurementType</v>
       </c>
       <c r="C63" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D63" t="s">
         <v>269</v>
-      </c>
-      <c r="D63" t="s">
-        <v>270</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -4111,10 +4226,10 @@
         <v>measurementType</v>
       </c>
       <c r="C64" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D64" t="s">
         <v>271</v>
-      </c>
-      <c r="D64" t="s">
-        <v>272</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -4133,7 +4248,7 @@
         <v>500</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>273</v>
+        <v>346</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -4152,7 +4267,7 @@
         <v>501</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -4171,7 +4286,7 @@
         <v>502</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -4190,7 +4305,7 @@
         <v>503</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -4209,7 +4324,7 @@
         <v>504</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -4228,7 +4343,7 @@
         <v>506</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -4247,7 +4362,7 @@
         <v>507</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -4266,7 +4381,7 @@
         <v>508</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -4285,7 +4400,7 @@
         <v>509</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -4304,7 +4419,7 @@
         <v>510</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -4323,7 +4438,7 @@
         <v>511</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
@@ -4342,7 +4457,7 @@
         <v>512</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -4361,7 +4476,7 @@
         <v>513</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -4380,7 +4495,7 @@
         <v>514</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -4399,7 +4514,7 @@
         <v>515</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E79" t="s">
         <v>13</v>
@@ -4418,7 +4533,7 @@
         <v>516</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E80" t="s">
         <v>13</v>
@@ -4437,7 +4552,7 @@
         <v>517</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
@@ -4456,7 +4571,7 @@
         <v>518</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E82" t="s">
         <v>13</v>
@@ -4475,7 +4590,7 @@
         <v>519</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E83" t="s">
         <v>13</v>
@@ -4494,7 +4609,7 @@
         <v>520</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E84" t="s">
         <v>13</v>
@@ -4513,7 +4628,7 @@
         <v>522</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -4532,7 +4647,7 @@
         <v>523</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>13</v>
@@ -4551,7 +4666,7 @@
         <v>524</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E87" t="s">
         <v>13</v>
@@ -4570,7 +4685,7 @@
         <v>525</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E88" t="s">
         <v>13</v>
@@ -4589,7 +4704,7 @@
         <v>526</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E89" t="s">
         <v>13</v>
@@ -4608,7 +4723,7 @@
         <v>527</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E90" t="s">
         <v>13</v>
@@ -4627,7 +4742,7 @@
         <v>528</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E91" t="s">
         <v>13</v>
@@ -4636,7 +4751,7 @@
     </row>
     <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B92" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4646,7 +4761,7 @@
         <v>401</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>13</v>
@@ -4655,7 +4770,7 @@
     </row>
     <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4665,7 +4780,7 @@
         <v>201</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>13</v>
@@ -4674,7 +4789,7 @@
     </row>
     <row r="94" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B94" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4684,7 +4799,7 @@
         <v>202</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>13</v>
@@ -4693,7 +4808,7 @@
     </row>
     <row r="95" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B95" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4703,7 +4818,7 @@
         <v>203</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>13</v>
@@ -4712,7 +4827,7 @@
     </row>
     <row r="96" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B96" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4722,7 +4837,7 @@
         <v>205</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>13</v>
@@ -4731,7 +4846,7 @@
     </row>
     <row r="97" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B97" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4741,7 +4856,7 @@
         <v>206</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>13</v>
@@ -4750,7 +4865,7 @@
     </row>
     <row r="98" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B98" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4760,7 +4875,7 @@
         <v>301</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>13</v>
@@ -4769,7 +4884,7 @@
     </row>
     <row r="99" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B99" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4779,7 +4894,7 @@
         <v>302</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E99" s="9" t="s">
         <v>13</v>
@@ -4788,7 +4903,7 @@
     </row>
     <row r="100" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B100" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4798,7 +4913,7 @@
         <v>303</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E100" s="9" t="s">
         <v>13</v>
@@ -4807,7 +4922,7 @@
     </row>
     <row r="101" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B101" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4817,7 +4932,7 @@
         <v>304</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>13</v>
@@ -4826,7 +4941,7 @@
     </row>
     <row r="102" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B102" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4836,7 +4951,7 @@
         <v>305</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>13</v>
@@ -4845,7 +4960,7 @@
     </row>
     <row r="103" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B103" s="1" t="str">
         <f>MetadataDict!$B$37</f>
@@ -4855,7 +4970,7 @@
         <v>306</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E103" s="9" t="s">
         <v>13</v>
@@ -4864,7 +4979,7 @@
     </row>
     <row r="104" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>119</v>
@@ -4873,7 +4988,7 @@
         <v>34</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E104" s="9" t="s">
         <v>13</v>
@@ -4882,7 +4997,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B105" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4892,7 +5007,7 @@
         <v>500</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E105" t="s">
         <v>13</v>
@@ -4900,7 +5015,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B106" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4910,7 +5025,7 @@
         <v>501</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E106" t="s">
         <v>13</v>
@@ -4918,7 +5033,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B107" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4928,7 +5043,7 @@
         <v>502</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E107" t="s">
         <v>13</v>
@@ -4936,7 +5051,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B108" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4946,7 +5061,7 @@
         <v>503</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E108" t="s">
         <v>13</v>
@@ -4954,7 +5069,7 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B109" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4964,7 +5079,7 @@
         <v>504</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E109" t="s">
         <v>13</v>
@@ -4972,7 +5087,7 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B110" t="str">
         <f>MetadataDict!$B$39</f>
@@ -4982,7 +5097,7 @@
         <v>506</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E110" t="s">
         <v>13</v>
@@ -4990,7 +5105,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B111" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5000,7 +5115,7 @@
         <v>507</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E111" t="s">
         <v>13</v>
@@ -5008,7 +5123,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B112" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5018,7 +5133,7 @@
         <v>508</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E112" t="s">
         <v>13</v>
@@ -5026,7 +5141,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B113" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5036,7 +5151,7 @@
         <v>509</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E113" t="s">
         <v>13</v>
@@ -5044,7 +5159,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B114" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5054,7 +5169,7 @@
         <v>510</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E114" t="s">
         <v>13</v>
@@ -5062,7 +5177,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B115" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5072,7 +5187,7 @@
         <v>511</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E115" t="s">
         <v>13</v>
@@ -5080,7 +5195,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B116" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5090,7 +5205,7 @@
         <v>512</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E116" t="s">
         <v>13</v>
@@ -5098,7 +5213,7 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B117" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5108,7 +5223,7 @@
         <v>513</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E117" t="s">
         <v>13</v>
@@ -5116,7 +5231,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B118" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5126,7 +5241,7 @@
         <v>514</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E118" t="s">
         <v>13</v>
@@ -5134,7 +5249,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B119" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5144,7 +5259,7 @@
         <v>515</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E119" t="s">
         <v>13</v>
@@ -5152,7 +5267,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B120" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5162,7 +5277,7 @@
         <v>516</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E120" t="s">
         <v>13</v>
@@ -5170,7 +5285,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B121" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5180,7 +5295,7 @@
         <v>517</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E121" t="s">
         <v>13</v>
@@ -5188,7 +5303,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5198,7 +5313,7 @@
         <v>518</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E122" t="s">
         <v>13</v>
@@ -5206,7 +5321,7 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5216,7 +5331,7 @@
         <v>519</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E123" t="s">
         <v>13</v>
@@ -5224,7 +5339,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B124" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5234,7 +5349,7 @@
         <v>520</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E124" t="s">
         <v>13</v>
@@ -5242,7 +5357,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B125" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5252,7 +5367,7 @@
         <v>522</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E125" t="s">
         <v>13</v>
@@ -5260,7 +5375,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5270,7 +5385,7 @@
         <v>523</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E126" t="s">
         <v>13</v>
@@ -5278,7 +5393,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5288,7 +5403,7 @@
         <v>524</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E127" t="s">
         <v>13</v>
@@ -5296,7 +5411,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5306,7 +5421,7 @@
         <v>525</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E128" t="s">
         <v>13</v>
@@ -5314,7 +5429,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B129" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5324,7 +5439,7 @@
         <v>526</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E129" t="s">
         <v>13</v>
@@ -5332,7 +5447,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B130" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5342,7 +5457,7 @@
         <v>527</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E130" t="s">
         <v>13</v>
@@ -5350,7 +5465,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B131" t="str">
         <f>MetadataDict!$B$39</f>
@@ -5360,7 +5475,7 @@
         <v>528</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E131" t="s">
         <v>13</v>
@@ -5368,7 +5483,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B132" t="s">
         <v>116</v>
@@ -5377,7 +5492,7 @@
         <v>22</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E132" t="s">
         <v>13</v>
@@ -5385,17 +5500,17 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B133" t="str">
         <f>MetadataDict!$B$41</f>
         <v>dataType</v>
       </c>
       <c r="C133" t="s">
+        <v>311</v>
+      </c>
+      <c r="D133" t="s">
         <v>312</v>
-      </c>
-      <c r="D133" t="s">
-        <v>313</v>
       </c>
       <c r="E133" t="s">
         <v>13</v>
@@ -5403,7 +5518,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B134" t="str">
         <f>MetadataDict!$B$41</f>
@@ -5413,7 +5528,7 @@
         <v>17</v>
       </c>
       <c r="D134" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E134" t="s">
         <v>13</v>
@@ -5421,17 +5536,17 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B135" t="str">
         <f>MetadataDict!$B$41</f>
         <v>dataType</v>
       </c>
       <c r="C135" t="s">
+        <v>314</v>
+      </c>
+      <c r="D135" t="s">
         <v>315</v>
-      </c>
-      <c r="D135" t="s">
-        <v>316</v>
       </c>
       <c r="E135" t="s">
         <v>13</v>
@@ -5439,7 +5554,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B136" t="str">
         <f>MetadataDict!$B$41</f>
@@ -5449,7 +5564,7 @@
         <v>24</v>
       </c>
       <c r="D136" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E136" t="s">
         <v>13</v>
@@ -5457,17 +5572,17 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B137" t="str">
         <f>MetadataDict!$B$42</f>
         <v>program</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E137" t="s">
         <v>13</v>
@@ -5475,17 +5590,17 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B138" t="str">
         <f>MetadataDict!$B$42</f>
         <v>program</v>
       </c>
       <c r="C138" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D138" t="s">
         <v>190</v>
-      </c>
-      <c r="D138" t="s">
-        <v>191</v>
       </c>
       <c r="E138" t="s">
         <v>13</v>
@@ -5493,17 +5608,17 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B139" t="str">
         <f>MetadataDict!$B$42</f>
         <v>program</v>
       </c>
       <c r="C139" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D139" t="s">
         <v>192</v>
-      </c>
-      <c r="D139" t="s">
-        <v>193</v>
       </c>
       <c r="E139" t="s">
         <v>13</v>
@@ -5511,17 +5626,17 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B140" t="str">
         <f>MetadataDict!$B$42</f>
         <v>program</v>
       </c>
       <c r="C140" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D140" t="s">
         <v>194</v>
-      </c>
-      <c r="D140" t="s">
-        <v>195</v>
       </c>
       <c r="E140" t="s">
         <v>13</v>
@@ -5529,16 +5644,16 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B141" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C141" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E141" t="s">
         <v>13</v>
@@ -5546,17 +5661,17 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B142" t="str">
         <f>MetadataDict!$B$45</f>
         <v>originalDataType</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E142" t="s">
         <v>13</v>
@@ -5564,17 +5679,17 @@
     </row>
     <row r="143" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B143" t="str">
         <f>MetadataDict!$B$45</f>
         <v>originalDataType</v>
       </c>
       <c r="C143" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="E143" t="s">
         <v>13</v>
@@ -5583,7 +5698,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B144" t="str">
         <f>MetadataDict!$B$45</f>
@@ -5593,7 +5708,7 @@
         <v>17</v>
       </c>
       <c r="D144" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E144" t="s">
         <v>13</v>
@@ -5601,7 +5716,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B145" t="str">
         <f>MetadataDict!$B$45</f>
@@ -5611,7 +5726,7 @@
         <v>24</v>
       </c>
       <c r="D145" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E145" t="s">
         <v>13</v>
@@ -5619,16 +5734,16 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E146" t="s">
         <v>13</v>
@@ -5636,16 +5751,16 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B147" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D147" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E147" t="s">
         <v>13</v>
@@ -5653,7 +5768,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B148" t="str">
         <f>MetadataDict!$B$50</f>
@@ -5663,7 +5778,7 @@
         <v>401</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E148" t="s">
         <v>13</v>
@@ -5672,7 +5787,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B149" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5682,7 +5797,7 @@
         <v>500</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E149" t="s">
         <v>13</v>
@@ -5690,7 +5805,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B150" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5700,7 +5815,7 @@
         <v>501</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E150" t="s">
         <v>13</v>
@@ -5709,7 +5824,7 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B151" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5719,7 +5834,7 @@
         <v>502</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E151" t="s">
         <v>13</v>
@@ -5728,7 +5843,7 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B152" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5738,7 +5853,7 @@
         <v>503</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E152" t="s">
         <v>13</v>
@@ -5747,7 +5862,7 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B153" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5757,7 +5872,7 @@
         <v>504</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E153" t="s">
         <v>13</v>
@@ -5766,7 +5881,7 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B154" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5776,7 +5891,7 @@
         <v>505</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E154" t="s">
         <v>13</v>
@@ -5785,7 +5900,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5795,7 +5910,7 @@
         <v>506</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E155" t="s">
         <v>13</v>
@@ -5804,7 +5919,7 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5814,7 +5929,7 @@
         <v>507</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E156" t="s">
         <v>13</v>
@@ -5823,7 +5938,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B157" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5833,7 +5948,7 @@
         <v>508</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E157" t="s">
         <v>13</v>
@@ -5842,7 +5957,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B158" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5852,7 +5967,7 @@
         <v>509</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E158" t="s">
         <v>13</v>
@@ -5861,7 +5976,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B159" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5871,7 +5986,7 @@
         <v>510</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E159" t="s">
         <v>13</v>
@@ -5880,7 +5995,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B160" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5890,7 +6005,7 @@
         <v>511</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E160" t="s">
         <v>13</v>
@@ -5899,7 +6014,7 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B161" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5909,7 +6024,7 @@
         <v>512</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E161" t="s">
         <v>13</v>
@@ -5918,7 +6033,7 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B162" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5928,7 +6043,7 @@
         <v>513</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E162" t="s">
         <v>13</v>
@@ -5937,7 +6052,7 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B163" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5947,7 +6062,7 @@
         <v>514</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E163" t="s">
         <v>13</v>
@@ -5956,7 +6071,7 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B164" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5966,7 +6081,7 @@
         <v>515</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E164" t="s">
         <v>13</v>
@@ -5975,7 +6090,7 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B165" t="str">
         <f>MetadataDict!$B$52</f>
@@ -5985,7 +6100,7 @@
         <v>516</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E165" t="s">
         <v>13</v>
@@ -5993,7 +6108,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B166" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6003,7 +6118,7 @@
         <v>517</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E166" t="s">
         <v>13</v>
@@ -6011,7 +6126,7 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B167" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6021,7 +6136,7 @@
         <v>518</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E167" t="s">
         <v>13</v>
@@ -6029,7 +6144,7 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B168" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6039,7 +6154,7 @@
         <v>519</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E168" t="s">
         <v>13</v>
@@ -6047,7 +6162,7 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B169" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6057,7 +6172,7 @@
         <v>520</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E169" t="s">
         <v>13</v>
@@ -6065,7 +6180,7 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B170" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6075,7 +6190,7 @@
         <v>522</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E170" t="s">
         <v>13</v>
@@ -6083,7 +6198,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B171" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6093,7 +6208,7 @@
         <v>523</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E171" t="s">
         <v>13</v>
@@ -6102,7 +6217,7 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B172" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6112,7 +6227,7 @@
         <v>524</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E172" t="s">
         <v>13</v>
@@ -6121,7 +6236,7 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B173" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6131,7 +6246,7 @@
         <v>525</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E173" t="s">
         <v>13</v>
@@ -6140,7 +6255,7 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B174" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6150,7 +6265,7 @@
         <v>526</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E174" t="s">
         <v>13</v>
@@ -6159,7 +6274,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B175" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6169,7 +6284,7 @@
         <v>527</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E175" t="s">
         <v>13</v>
@@ -6178,7 +6293,7 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B176" t="str">
         <f>MetadataDict!$B$52</f>
@@ -6188,47 +6303,47 @@
         <v>528</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E176" t="s">
         <v>13</v>
       </c>
       <c r="F176" s="4"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B177" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C177" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D177" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D177" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="E177" t="s">
         <v>13</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B178" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C178" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D178" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="E178" t="s">
         <v>13</v>
@@ -6236,461 +6351,530 @@
       <c r="F178" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G178">
+        <v>1</v>
+      </c>
+      <c r="H178">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B179" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D179" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E179" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="E179" t="s">
-        <v>13</v>
-      </c>
-      <c r="F179" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B180" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C180" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D180" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D180" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="E180" t="s">
         <v>13</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B181" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C181" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D181" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D181" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="E181" t="s">
         <v>13</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B182" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C182" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D182" t="s">
         <v>327</v>
       </c>
-      <c r="D182" t="s">
+      <c r="E182" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="E182" t="s">
-        <v>13</v>
-      </c>
-      <c r="F182" s="4" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B183" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C183" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D183" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D183" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="E183" t="s">
         <v>13</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
+      <c r="H183">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B184" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E184" t="s">
         <v>13</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B185" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C185" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D185" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D185" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="E185" t="s">
         <v>13</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B186" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C186" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D186" t="s">
         <v>235</v>
       </c>
-      <c r="D186" t="s">
-        <v>236</v>
-      </c>
       <c r="E186" t="s">
         <v>13</v>
       </c>
       <c r="F186" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B187" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C187" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D187" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D187" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="E187" t="s">
         <v>13</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G187">
+        <v>0</v>
+      </c>
+      <c r="H187">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B188" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C188" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D188" t="s">
         <v>239</v>
       </c>
-      <c r="D188" t="s">
-        <v>240</v>
-      </c>
       <c r="E188" t="s">
         <v>13</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B189" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C189" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D189" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D189" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="E189" t="s">
         <v>13</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B190" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C190" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D190" t="s">
         <v>243</v>
       </c>
-      <c r="D190" t="s">
-        <v>244</v>
-      </c>
       <c r="E190" t="s">
         <v>13</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B191" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C191" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D191" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D191" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E191" t="s">
         <v>13</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
+      <c r="H191">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B192" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C192" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D192" t="s">
         <v>247</v>
       </c>
-      <c r="D192" t="s">
-        <v>248</v>
-      </c>
       <c r="E192" t="s">
         <v>13</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
+      <c r="H192">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B193" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C193" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D193" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D193" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="E193" t="s">
         <v>13</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B194" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C194" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="D194" t="s">
         <v>251</v>
       </c>
-      <c r="D194" t="s">
-        <v>252</v>
-      </c>
       <c r="E194" t="s">
         <v>13</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
+      <c r="H194">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B195" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C195" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D195" t="s">
         <v>253</v>
       </c>
-      <c r="D195" t="s">
-        <v>254</v>
-      </c>
       <c r="E195" t="s">
         <v>13</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B196" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C196" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D196" t="s">
         <v>255</v>
       </c>
-      <c r="D196" t="s">
-        <v>256</v>
-      </c>
       <c r="E196" t="s">
         <v>13</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
+      <c r="H196">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B197" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C197" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D197" t="s">
         <v>257</v>
       </c>
-      <c r="D197" t="s">
-        <v>258</v>
-      </c>
       <c r="E197" t="s">
         <v>13</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G197">
+        <v>0</v>
+      </c>
+      <c r="H197">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B198" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C198" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D198" t="s">
         <v>259</v>
       </c>
-      <c r="D198" t="s">
-        <v>260</v>
-      </c>
       <c r="E198" t="s">
         <v>13</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+      <c r="H198">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B199" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C199" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D199" t="s">
         <v>261</v>
       </c>
-      <c r="D199" t="s">
-        <v>262</v>
-      </c>
       <c r="E199" t="s">
         <v>13</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B200" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D200" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E200" t="s">
         <v>13</v>
@@ -6698,157 +6882,163 @@
       <c r="F200" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G200">
+        <v>0</v>
+      </c>
+      <c r="H200">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B201" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C201" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D201" t="s">
         <v>265</v>
       </c>
-      <c r="D201" t="s">
-        <v>266</v>
-      </c>
       <c r="E201" t="s">
         <v>13</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B202" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C202" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D202" t="s">
         <v>267</v>
       </c>
-      <c r="D202" t="s">
-        <v>268</v>
-      </c>
       <c r="E202" t="s">
         <v>13</v>
       </c>
       <c r="F202" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B203" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C203" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D203" t="s">
         <v>269</v>
       </c>
-      <c r="D203" t="s">
-        <v>270</v>
-      </c>
       <c r="E203" t="s">
         <v>13</v>
       </c>
       <c r="F203" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B204" t="str">
         <f>MetadataDict!$B$53</f>
         <v>measurementType</v>
       </c>
       <c r="C204" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D204" t="s">
         <v>271</v>
       </c>
-      <c r="D204" t="s">
-        <v>272</v>
-      </c>
       <c r="E204" t="s">
         <v>13</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B205" t="str">
         <f>MetadataDict!$B$56</f>
         <v>dataType</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D205" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E205" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B206" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D206" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E206" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B207" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D207" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E207" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B208" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C208" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D208" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E208" t="s">
         <v>13</v>
@@ -6856,17 +7046,17 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B209" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C209" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D209" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E209" t="s">
         <v>13</v>
@@ -6874,17 +7064,17 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B210" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C210" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D210" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E210" t="s">
         <v>13</v>
@@ -6892,17 +7082,17 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B211" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C211" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D211" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E211" t="s">
         <v>13</v>
@@ -6910,17 +7100,17 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B212" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C212" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D212" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E212" t="s">
         <v>13</v>
@@ -6928,17 +7118,17 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B213" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C213" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D213" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E213" t="s">
         <v>13</v>
@@ -6946,17 +7136,17 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B214" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C214" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D214" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E214" t="s">
         <v>13</v>
@@ -6964,17 +7154,17 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B215" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C215" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D215" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E215" t="s">
         <v>13</v>
@@ -6982,17 +7172,17 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B216" t="str">
         <f>MetadataDict!$B$55</f>
         <v>unit</v>
       </c>
       <c r="C216" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D216" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E216" t="s">
         <v>13</v>
@@ -7000,16 +7190,16 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B217" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C217" t="s">
         <v>34</v>
       </c>
       <c r="D217" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E217" t="s">
         <v>13</v>
@@ -7017,16 +7207,16 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B218" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C218" t="s">
         <v>34</v>
       </c>
       <c r="D218" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E218" t="s">
         <v>13</v>
@@ -7042,6 +7232,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006688A6CBE26CBF41BFE362BEC34502BA" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="916ec95d980b70225c2beeb175eb34ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xmlns:ns3="3618cbaa-901d-4c6b-9f1a-f53e3aa15701" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1086361ad164fb1fc8fad31a5b69396c" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7279,7 +7478,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -7290,16 +7489,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783B9ED7-A86D-4C20-8581-4B66EC9EBDC7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7319,7 +7517,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -7328,12 +7526,4 @@
     <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update to use MetadataDictionary as system of record
</commit_message>
<xml_diff>
--- a/Data/MetadataDictionary.xlsx
+++ b/Data/MetadataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rscully\Documents\Projects\Habitat Data Sharing\2019_2020\Code\Stream-Monitoring-Data-Exchange-Specifications\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BEE017-D0F1-4E16-AF52-B5BA3E92F075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED25F33-0015-423D-A12A-FCB6CDBCB1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-4305" windowWidth="38640" windowHeight="21240" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
+    <workbookView xWindow="-38520" yWindow="-4305" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{612D857E-CB7D-4F80-AB73-368B543E7FF3}"/>
   </bookViews>
   <sheets>
     <sheet name="MetadataDict" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="350">
   <si>
     <t>entity</t>
   </si>
@@ -851,9 +851,6 @@
   </si>
   <si>
     <t>Average water clarity as measured by the suspended solids in the water column (unit: NTU or Nephelometric Turbidity unit)</t>
-  </si>
-  <si>
-    <t>A unique numeric identifier assigned to measurementType Sin.</t>
   </si>
   <si>
     <t>A unique numeric identifier assigned to the measurementType StreamOrder.</t>
@@ -1512,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E6029B-A891-4391-9A91-8B6BC1C75C07}">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
@@ -1572,18 +1569,18 @@
         <v>135</v>
       </c>
       <c r="M1" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>348</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -1596,7 +1593,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1655,7 +1652,7 @@
     </row>
     <row r="5" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -1687,7 +1684,7 @@
     </row>
     <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -1722,7 +1719,7 @@
     </row>
     <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -1751,7 +1748,7 @@
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -1777,7 +1774,7 @@
     </row>
     <row r="9" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
@@ -1809,7 +1806,7 @@
     </row>
     <row r="10" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
@@ -1836,9 +1833,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -1865,7 +1862,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="203" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -1876,7 +1873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -1899,7 +1896,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -1992,7 +1989,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2024,7 +2021,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2050,7 +2047,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2085,7 +2082,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -2128,7 +2125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -2154,7 +2151,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -2192,7 +2189,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="145" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -2224,7 +2221,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -2326,7 +2323,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2393,7 +2390,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -2404,7 +2401,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="145" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -2433,7 +2430,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -2462,7 +2459,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -2511,7 +2508,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -2540,7 +2537,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -3044,9 +3041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063D4566-F61A-451E-B178-010037E4B35B}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4248,7 +4245,7 @@
         <v>500</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -4267,7 +4264,7 @@
         <v>501</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -4286,7 +4283,7 @@
         <v>502</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -4305,7 +4302,7 @@
         <v>503</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -4324,7 +4321,7 @@
         <v>504</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -4343,7 +4340,7 @@
         <v>506</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -4362,7 +4359,7 @@
         <v>507</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -4381,7 +4378,7 @@
         <v>508</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -4400,7 +4397,7 @@
         <v>509</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -4419,7 +4416,7 @@
         <v>510</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -4438,7 +4435,7 @@
         <v>511</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
@@ -4457,7 +4454,7 @@
         <v>512</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -4476,7 +4473,7 @@
         <v>513</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -4495,7 +4492,7 @@
         <v>514</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -4514,7 +4511,7 @@
         <v>515</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E79" t="s">
         <v>13</v>
@@ -4533,7 +4530,7 @@
         <v>516</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E80" t="s">
         <v>13</v>
@@ -4552,7 +4549,7 @@
         <v>517</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
@@ -4571,7 +4568,7 @@
         <v>518</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E82" t="s">
         <v>13</v>
@@ -4590,7 +4587,7 @@
         <v>519</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E83" t="s">
         <v>13</v>
@@ -4609,7 +4606,7 @@
         <v>520</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E84" t="s">
         <v>13</v>
@@ -4628,7 +4625,7 @@
         <v>522</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -4647,7 +4644,7 @@
         <v>523</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>13</v>
@@ -4666,7 +4663,7 @@
         <v>524</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E87" t="s">
         <v>13</v>
@@ -4685,7 +4682,7 @@
         <v>525</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E88" t="s">
         <v>13</v>
@@ -4704,7 +4701,7 @@
         <v>526</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E89" t="s">
         <v>13</v>
@@ -4723,7 +4720,7 @@
         <v>527</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E90" t="s">
         <v>13</v>
@@ -4742,7 +4739,7 @@
         <v>528</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E91" t="s">
         <v>13</v>
@@ -4761,7 +4758,7 @@
         <v>401</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E92" s="9" t="s">
         <v>13</v>
@@ -4780,7 +4777,7 @@
         <v>201</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E93" s="9" t="s">
         <v>13</v>
@@ -4799,7 +4796,7 @@
         <v>202</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E94" s="9" t="s">
         <v>13</v>
@@ -4818,7 +4815,7 @@
         <v>203</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E95" s="9" t="s">
         <v>13</v>
@@ -4837,7 +4834,7 @@
         <v>205</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E96" s="9" t="s">
         <v>13</v>
@@ -4856,7 +4853,7 @@
         <v>206</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E97" s="9" t="s">
         <v>13</v>
@@ -4875,7 +4872,7 @@
         <v>301</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E98" s="9" t="s">
         <v>13</v>
@@ -4894,7 +4891,7 @@
         <v>302</v>
       </c>
       <c r="D99" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E99" s="9" t="s">
         <v>13</v>
@@ -4913,7 +4910,7 @@
         <v>303</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E100" s="9" t="s">
         <v>13</v>
@@ -4932,7 +4929,7 @@
         <v>304</v>
       </c>
       <c r="D101" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E101" s="9" t="s">
         <v>13</v>
@@ -4951,7 +4948,7 @@
         <v>305</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E102" s="9" t="s">
         <v>13</v>
@@ -4970,7 +4967,7 @@
         <v>306</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E103" s="9" t="s">
         <v>13</v>
@@ -5007,7 +5004,7 @@
         <v>500</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E105" t="s">
         <v>13</v>
@@ -5025,7 +5022,7 @@
         <v>501</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E106" t="s">
         <v>13</v>
@@ -5043,7 +5040,7 @@
         <v>502</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E107" t="s">
         <v>13</v>
@@ -5061,7 +5058,7 @@
         <v>503</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E108" t="s">
         <v>13</v>
@@ -5079,7 +5076,7 @@
         <v>504</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E109" t="s">
         <v>13</v>
@@ -5097,7 +5094,7 @@
         <v>506</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E110" t="s">
         <v>13</v>
@@ -5115,7 +5112,7 @@
         <v>507</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E111" t="s">
         <v>13</v>
@@ -5133,7 +5130,7 @@
         <v>508</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E112" t="s">
         <v>13</v>
@@ -5151,7 +5148,7 @@
         <v>509</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E113" t="s">
         <v>13</v>
@@ -5169,7 +5166,7 @@
         <v>510</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E114" t="s">
         <v>13</v>
@@ -5187,7 +5184,7 @@
         <v>511</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E115" t="s">
         <v>13</v>
@@ -5205,7 +5202,7 @@
         <v>512</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E116" t="s">
         <v>13</v>
@@ -5223,7 +5220,7 @@
         <v>513</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E117" t="s">
         <v>13</v>
@@ -5241,7 +5238,7 @@
         <v>514</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E118" t="s">
         <v>13</v>
@@ -5259,7 +5256,7 @@
         <v>515</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E119" t="s">
         <v>13</v>
@@ -5277,7 +5274,7 @@
         <v>516</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E120" t="s">
         <v>13</v>
@@ -5295,7 +5292,7 @@
         <v>517</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E121" t="s">
         <v>13</v>
@@ -5313,7 +5310,7 @@
         <v>518</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E122" t="s">
         <v>13</v>
@@ -5331,7 +5328,7 @@
         <v>519</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E123" t="s">
         <v>13</v>
@@ -5349,7 +5346,7 @@
         <v>520</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E124" t="s">
         <v>13</v>
@@ -5367,7 +5364,7 @@
         <v>522</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E125" t="s">
         <v>13</v>
@@ -5385,7 +5382,7 @@
         <v>523</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E126" t="s">
         <v>13</v>
@@ -5403,7 +5400,7 @@
         <v>524</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E127" t="s">
         <v>13</v>
@@ -5421,7 +5418,7 @@
         <v>525</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E128" t="s">
         <v>13</v>
@@ -5439,7 +5436,7 @@
         <v>526</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E129" t="s">
         <v>13</v>
@@ -5457,7 +5454,7 @@
         <v>527</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E130" t="s">
         <v>13</v>
@@ -5475,7 +5472,7 @@
         <v>528</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E131" t="s">
         <v>13</v>
@@ -5507,10 +5504,10 @@
         <v>dataType</v>
       </c>
       <c r="C133" t="s">
+        <v>310</v>
+      </c>
+      <c r="D133" t="s">
         <v>311</v>
-      </c>
-      <c r="D133" t="s">
-        <v>312</v>
       </c>
       <c r="E133" t="s">
         <v>13</v>
@@ -5528,7 +5525,7 @@
         <v>17</v>
       </c>
       <c r="D134" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E134" t="s">
         <v>13</v>
@@ -5543,10 +5540,10 @@
         <v>dataType</v>
       </c>
       <c r="C135" t="s">
+        <v>313</v>
+      </c>
+      <c r="D135" t="s">
         <v>314</v>
-      </c>
-      <c r="D135" t="s">
-        <v>315</v>
       </c>
       <c r="E135" t="s">
         <v>13</v>
@@ -5564,7 +5561,7 @@
         <v>24</v>
       </c>
       <c r="D136" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E136" t="s">
         <v>13</v>
@@ -5582,7 +5579,7 @@
         <v>187</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E137" t="s">
         <v>13</v>
@@ -5668,10 +5665,10 @@
         <v>originalDataType</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E142" t="s">
         <v>13</v>
@@ -5686,10 +5683,10 @@
         <v>originalDataType</v>
       </c>
       <c r="C143" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D143" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="E143" t="s">
         <v>13</v>
@@ -5708,7 +5705,7 @@
         <v>17</v>
       </c>
       <c r="D144" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E144" t="s">
         <v>13</v>
@@ -5726,7 +5723,7 @@
         <v>24</v>
       </c>
       <c r="D145" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E145" t="s">
         <v>13</v>
@@ -5778,7 +5775,7 @@
         <v>401</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E148" t="s">
         <v>13</v>
@@ -5797,7 +5794,7 @@
         <v>500</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>272</v>
+        <v>345</v>
       </c>
       <c r="E149" t="s">
         <v>13</v>
@@ -5815,7 +5812,7 @@
         <v>501</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E150" t="s">
         <v>13</v>
@@ -5834,7 +5831,7 @@
         <v>502</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E151" t="s">
         <v>13</v>
@@ -5853,7 +5850,7 @@
         <v>503</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E152" t="s">
         <v>13</v>
@@ -5872,7 +5869,7 @@
         <v>504</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E153" t="s">
         <v>13</v>
@@ -5891,7 +5888,7 @@
         <v>505</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E154" t="s">
         <v>13</v>
@@ -5910,7 +5907,7 @@
         <v>506</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E155" t="s">
         <v>13</v>
@@ -5929,7 +5926,7 @@
         <v>507</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E156" t="s">
         <v>13</v>
@@ -5948,7 +5945,7 @@
         <v>508</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E157" t="s">
         <v>13</v>
@@ -5967,7 +5964,7 @@
         <v>509</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E158" t="s">
         <v>13</v>
@@ -5986,7 +5983,7 @@
         <v>510</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E159" t="s">
         <v>13</v>
@@ -6005,7 +6002,7 @@
         <v>511</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E160" t="s">
         <v>13</v>
@@ -6024,7 +6021,7 @@
         <v>512</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E161" t="s">
         <v>13</v>
@@ -6043,7 +6040,7 @@
         <v>513</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E162" t="s">
         <v>13</v>
@@ -6062,7 +6059,7 @@
         <v>514</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E163" t="s">
         <v>13</v>
@@ -6081,7 +6078,7 @@
         <v>515</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E164" t="s">
         <v>13</v>
@@ -6100,7 +6097,7 @@
         <v>516</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E165" t="s">
         <v>13</v>
@@ -6118,7 +6115,7 @@
         <v>517</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E166" t="s">
         <v>13</v>
@@ -6136,7 +6133,7 @@
         <v>518</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E167" t="s">
         <v>13</v>
@@ -6154,7 +6151,7 @@
         <v>519</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E168" t="s">
         <v>13</v>
@@ -6172,7 +6169,7 @@
         <v>520</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E169" t="s">
         <v>13</v>
@@ -6190,7 +6187,7 @@
         <v>522</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E170" t="s">
         <v>13</v>
@@ -6208,7 +6205,7 @@
         <v>523</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E171" t="s">
         <v>13</v>
@@ -6227,7 +6224,7 @@
         <v>524</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E172" t="s">
         <v>13</v>
@@ -6246,7 +6243,7 @@
         <v>525</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E173" t="s">
         <v>13</v>
@@ -6265,7 +6262,7 @@
         <v>526</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E174" t="s">
         <v>13</v>
@@ -6284,7 +6281,7 @@
         <v>527</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E175" t="s">
         <v>13</v>
@@ -6303,7 +6300,7 @@
         <v>528</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E176" t="s">
         <v>13</v>
@@ -6328,7 +6325,7 @@
         <v>13</v>
       </c>
       <c r="F177" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -6370,13 +6367,13 @@
         <v>222</v>
       </c>
       <c r="D179" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E179" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="4" t="s">
         <v>324</v>
-      </c>
-      <c r="E179" t="s">
-        <v>13</v>
-      </c>
-      <c r="F179" s="4" t="s">
-        <v>325</v>
       </c>
       <c r="G179">
         <v>0</v>
@@ -6400,7 +6397,7 @@
         <v>13</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -6421,7 +6418,7 @@
         <v>13</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -6433,16 +6430,16 @@
         <v>measurementType</v>
       </c>
       <c r="C182" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D182" t="s">
         <v>326</v>
       </c>
-      <c r="D182" t="s">
+      <c r="E182" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="E182" t="s">
-        <v>13</v>
-      </c>
-      <c r="F182" s="4" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -6463,7 +6460,7 @@
         <v>13</v>
       </c>
       <c r="F183" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G183">
         <v>0</v>
@@ -6484,13 +6481,13 @@
         <v>230</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E184" t="s">
         <v>13</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
@@ -6511,7 +6508,7 @@
         <v>13</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -6532,7 +6529,7 @@
         <v>13</v>
       </c>
       <c r="F186" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -6553,7 +6550,7 @@
         <v>13</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G187">
         <v>0</v>
@@ -6580,7 +6577,7 @@
         <v>13</v>
       </c>
       <c r="F188" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -6601,7 +6598,7 @@
         <v>13</v>
       </c>
       <c r="F189" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -6622,7 +6619,7 @@
         <v>13</v>
       </c>
       <c r="F190" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
@@ -6643,7 +6640,7 @@
         <v>13</v>
       </c>
       <c r="F191" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -6670,7 +6667,7 @@
         <v>13</v>
       </c>
       <c r="F192" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G192">
         <v>0</v>
@@ -6697,7 +6694,7 @@
         <v>13</v>
       </c>
       <c r="F193" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G193">
         <v>0</v>
@@ -6724,7 +6721,7 @@
         <v>13</v>
       </c>
       <c r="F194" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G194">
         <v>0</v>
@@ -6751,7 +6748,7 @@
         <v>13</v>
       </c>
       <c r="F195" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G195">
         <v>0</v>
@@ -6778,7 +6775,7 @@
         <v>13</v>
       </c>
       <c r="F196" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G196">
         <v>0</v>
@@ -6805,7 +6802,7 @@
         <v>13</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G197">
         <v>0</v>
@@ -6832,7 +6829,7 @@
         <v>13</v>
       </c>
       <c r="F198" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G198">
         <v>0</v>
@@ -6859,7 +6856,7 @@
         <v>13</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
@@ -6874,7 +6871,7 @@
         <v>262</v>
       </c>
       <c r="D200" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E200" t="s">
         <v>13</v>
@@ -6907,7 +6904,7 @@
         <v>13</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
@@ -6928,7 +6925,7 @@
         <v>13</v>
       </c>
       <c r="F202" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
@@ -6949,7 +6946,7 @@
         <v>13</v>
       </c>
       <c r="F203" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
@@ -6970,7 +6967,7 @@
         <v>13</v>
       </c>
       <c r="F204" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
@@ -6982,10 +6979,10 @@
         <v>dataType</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D205" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E205" t="s">
         <v>13</v>
@@ -7017,10 +7014,10 @@
         <v>unit</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D207" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E207" t="s">
         <v>13</v>
@@ -7035,10 +7032,10 @@
         <v>unit</v>
       </c>
       <c r="C208" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D208" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E208" t="s">
         <v>13</v>
@@ -7053,10 +7050,10 @@
         <v>unit</v>
       </c>
       <c r="C209" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D209" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E209" t="s">
         <v>13</v>
@@ -7071,10 +7068,10 @@
         <v>unit</v>
       </c>
       <c r="C210" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D210" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E210" t="s">
         <v>13</v>
@@ -7089,10 +7086,10 @@
         <v>unit</v>
       </c>
       <c r="C211" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D211" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E211" t="s">
         <v>13</v>
@@ -7107,10 +7104,10 @@
         <v>unit</v>
       </c>
       <c r="C212" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D212" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E212" t="s">
         <v>13</v>
@@ -7125,10 +7122,10 @@
         <v>unit</v>
       </c>
       <c r="C213" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D213" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E213" t="s">
         <v>13</v>
@@ -7143,10 +7140,10 @@
         <v>unit</v>
       </c>
       <c r="C214" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D214" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E214" t="s">
         <v>13</v>
@@ -7161,10 +7158,10 @@
         <v>unit</v>
       </c>
       <c r="C215" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D215" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E215" t="s">
         <v>13</v>
@@ -7179,10 +7176,10 @@
         <v>unit</v>
       </c>
       <c r="C216" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D216" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E216" t="s">
         <v>13</v>
@@ -7232,12 +7229,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Number xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
+    <DateandTime xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7479,20 +7478,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Number xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
-    <DateandTime xmlns="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7518,12 +7518,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F29970C-55C3-4834-9A3F-8E46C108106D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06B41B24-566D-47DB-B2A1-8A240BF055D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e2c843f9-3b2b-47f3-8277-ec7d36bcd5c9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>